<commit_message>
Correction adresse du samedi
</commit_message>
<xml_diff>
--- a/content/static/Tarifs club JEEN 2022-2023.xlsx
+++ b/content/static/Tarifs club JEEN 2022-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DSV0000001.ap.cdc.fr\DFS_USERS$\numbachbascone\Perso\Prive\Prive\10 ECHECS\01 JEEN\30 ECHECS excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\michael\jeen-website\content\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C244DE6F-C6A0-4B36-9967-8528E21CF22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD142A1-1131-4F8F-B7AF-2A9B9481F846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-60" windowWidth="19440" windowHeight="15000" xr2:uid="{2C595CFA-FB7B-4B73-88BE-8CA4F377B685}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="12855" windowHeight="20940" xr2:uid="{2C595CFA-FB7B-4B73-88BE-8CA4F377B685}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
   <si>
     <t>jour</t>
   </si>
@@ -625,6 +625,9 @@
       </rPr>
       <t xml:space="preserve"> (versement en une ou plusieurs fois), le JÉEN délivre une attestation permettant de déduire directement de ses impôts 66% de la somme versée au club.</t>
     </r>
+  </si>
+  <si>
+    <t>53 rue Erlanger</t>
   </si>
 </sst>
 </file>
@@ -888,13 +891,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -929,7 +929,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -937,8 +937,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -948,7 +947,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -973,11 +971,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1775,7 +1772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311AF4F8-FF94-4D78-A485-EEF6C880521D}">
   <dimension ref="B3:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1786,726 +1785,685 @@
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="1.7109375" customWidth="1"/>
-    <col min="9" max="18" width="11.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="2:18" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="2:18" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="2:18" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+    <row r="3" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+      <c r="B5" s="16"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="2:18" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="2:18" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="2:18" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="24" t="s">
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="2:18" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-    </row>
-    <row r="14" spans="2:18" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29" t="s">
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="2:18" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22" t="s">
+      <c r="G14" s="23"/>
+      <c r="I14"/>
+      <c r="J14" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-    </row>
-    <row r="15" spans="2:18" s="27" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="2:18" s="19" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22">
+      <c r="I15"/>
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-    </row>
-    <row r="16" spans="2:18" s="27" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="32" t="s">
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+    </row>
+    <row r="16" spans="2:18" s="19" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22">
+      <c r="I16"/>
+      <c r="J16">
         <v>3</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-    </row>
-    <row r="17" spans="2:18" s="27" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="32" t="s">
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+    </row>
+    <row r="17" spans="2:18" s="19" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22">
+      <c r="I17"/>
+      <c r="J17">
         <v>4.5</v>
       </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-    </row>
-    <row r="18" spans="2:18" s="27" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="32" t="s">
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+    </row>
+    <row r="18" spans="2:18" s="19" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22">
+      <c r="I18"/>
+      <c r="J18">
         <v>4.5</v>
       </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-    </row>
-    <row r="19" spans="2:18" s="27" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="32" t="s">
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+    </row>
+    <row r="19" spans="2:18" s="19" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="33" t="s">
+      <c r="D19" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22">
+      <c r="I19"/>
+      <c r="J19">
         <v>3</v>
       </c>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="J20" s="21">
+      <c r="J20" s="18">
         <f>SUM(J15:J19)</f>
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:18" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-    </row>
-    <row r="23" spans="2:18" s="27" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="44" t="s">
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+    </row>
+    <row r="23" spans="2:18" s="19" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-    </row>
-    <row r="25" spans="2:18" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B25" s="39" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+    </row>
+    <row r="25" spans="2:18" s="34" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B25" s="33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="51" t="s">
+    <row r="26" spans="2:18" s="19" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="53"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-    </row>
-    <row r="27" spans="2:18" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="48" t="s">
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+    </row>
+    <row r="27" spans="2:18" s="19" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="50"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
     </row>
     <row r="29" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-    </row>
-    <row r="43" spans="2:18" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B43" s="44" t="s">
+    <row r="34" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="35"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+    </row>
+    <row r="43" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B43" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22"/>
-    </row>
-    <row r="44" spans="2:18" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-    </row>
-    <row r="45" spans="2:18" s="27" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="24" t="s">
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+    </row>
+    <row r="44" spans="2:18" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+    </row>
+    <row r="45" spans="2:18" s="19" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="25" t="s">
+      <c r="D45" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E45" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="35"/>
-      <c r="G45" s="24" t="s">
+      <c r="F45" s="30"/>
+      <c r="G45" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22" t="s">
+      <c r="I45"/>
+      <c r="J45" t="s">
         <v>52</v>
       </c>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="22"/>
-    </row>
-    <row r="46" spans="2:18" s="27" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="37" t="s">
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+    </row>
+    <row r="46" spans="2:18" s="19" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="33" t="s">
+      <c r="C46" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="54" t="s">
+      <c r="E46" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="33" t="s">
+      <c r="F46" s="49"/>
+      <c r="G46" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22">
+      <c r="I46"/>
+      <c r="J46">
         <v>1.5</v>
       </c>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-    </row>
-    <row r="47" spans="2:18" s="27" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="37" t="s">
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+    </row>
+    <row r="47" spans="2:18" s="19" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="54" t="s">
+      <c r="E47" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="55"/>
-      <c r="G47" s="33" t="s">
+      <c r="F47" s="49"/>
+      <c r="G47" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22">
+      <c r="I47"/>
+      <c r="J47">
         <v>1.5</v>
       </c>
-      <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="22"/>
-    </row>
-    <row r="48" spans="2:18" s="27" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="37" t="s">
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+    </row>
+    <row r="48" spans="2:18" s="19" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="33" t="s">
+      <c r="C48" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="54" t="s">
+      <c r="E48" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="F48" s="55"/>
-      <c r="G48" s="33" t="s">
+      <c r="F48" s="49"/>
+      <c r="G48" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22">
+      <c r="I48"/>
+      <c r="J48">
         <v>1.5</v>
       </c>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-    </row>
-    <row r="49" spans="2:18" s="27" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="37" t="s">
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+    </row>
+    <row r="49" spans="2:18" s="19" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="C49" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="54" t="s">
+      <c r="E49" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="F49" s="55"/>
-      <c r="G49" s="33" t="s">
+      <c r="F49" s="49"/>
+      <c r="G49" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22">
+      <c r="I49"/>
+      <c r="J49">
         <v>1.5</v>
       </c>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="22"/>
-    </row>
-    <row r="50" spans="2:18" s="27" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="37" t="s">
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+    </row>
+    <row r="50" spans="2:18" s="19" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="54" t="s">
+      <c r="E50" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="F50" s="55"/>
-      <c r="G50" s="33" t="s">
+      <c r="F50" s="49"/>
+      <c r="G50" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22">
+      <c r="I50"/>
+      <c r="J50">
         <v>1.5</v>
       </c>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="J51" s="21">
+      <c r="J51" s="18">
         <f>SUM(J46:J50)</f>
         <v>7.5</v>
       </c>
     </row>
     <row r="52" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="2:18" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="38" t="s">
+    <row r="53" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B53" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-    </row>
-    <row r="54" spans="2:18" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="36" t="s">
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+    </row>
+    <row r="54" spans="2:18" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-    </row>
-    <row r="56" spans="2:18" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="39" t="s">
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+    </row>
+    <row r="56" spans="2:18" s="34" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="2:18" s="36" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="45" t="s">
+    <row r="57" spans="2:18" s="2" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -2519,12 +2477,12 @@
     </row>
     <row r="58" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="60" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="37" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2567,175 +2525,172 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-  </cols>
   <sheetData>
     <row r="7" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D7" s="10"/>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D8" s="11"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="4:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="4:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="4:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="4:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="4:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="4:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="4:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="12" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>